<commit_message>
20h 27m before PA3PbIB O4KA by Polyakov
</commit_message>
<xml_diff>
--- a/Work/Output/BD_version_1.xlsx
+++ b/Work/Output/BD_version_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Desktop\Github\3BR-base\Output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\PycharmProjects\Polyakov\3BR-base\Work\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F8113B-AC58-4752-9BB4-98EBD8DF79E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69492FB1-C706-4E7F-BF5B-5B9E935D4FE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -163,7 +163,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -444,17 +444,17 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -477,7 +477,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -500,7 +500,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -523,7 +523,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -546,7 +546,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -569,7 +569,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -589,10 +589,10 @@
         <v>40</v>
       </c>
       <c r="G6">
-        <v>2550</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -615,7 +615,7 @@
         <v>2150</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -638,7 +638,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -661,7 +661,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -684,7 +684,7 @@
         <v>2350</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>

</xml_diff>